<commit_message>
fix regex in UIOperation.class
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10872" windowHeight="4968" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="4965" tabRatio="331"/>
   </bookViews>
   <sheets>
     <sheet name="UItests" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,19 +500,19 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -529,7 +529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -538,7 +538,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -551,7 +551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -568,7 +568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -583,7 +583,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -600,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -615,7 +615,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="7" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add ERR HANDL TC for items search functionality, refactoring
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10872" windowHeight="4968" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="4965" tabRatio="331"/>
   </bookViews>
   <sheets>
     <sheet name="UItests" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Keyword</t>
   </si>
@@ -46,36 +46,12 @@
     <t>VERIFYPAGETITLE</t>
   </si>
   <si>
-    <t>SCROLLINTOVIEW</t>
-  </si>
-  <si>
     <t>CLICK</t>
   </si>
   <si>
-    <t>dressesSection</t>
-  </si>
-  <si>
-    <t>Dresses - My Store</t>
-  </si>
-  <si>
-    <t>sliderMax</t>
-  </si>
-  <si>
     <t>http://automationpractice.com/index.php</t>
   </si>
   <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>pageItems</t>
-  </si>
-  <si>
-    <t>VERIFYPRICERANGE(MAX)</t>
-  </si>
-  <si>
-    <t>SETPRICERANGE(MAX)</t>
-  </si>
-  <si>
     <t>VERIFYBROKENLINKS</t>
   </si>
   <si>
@@ -88,16 +64,43 @@
     <t>images</t>
   </si>
   <si>
-    <t>TC # 01.05 - Use slider for setting price range (Max)</t>
-  </si>
-  <si>
-    <t>TC # 01.05</t>
+    <t>SETTEXTIN</t>
+  </si>
+  <si>
+    <t>searchField</t>
+  </si>
+  <si>
+    <t>searchButton</t>
+  </si>
+  <si>
+    <t>My Store</t>
+  </si>
+  <si>
+    <t>TC # 01.06 - Search can`t find results</t>
+  </si>
+  <si>
+    <t>~!@#$%^&amp;*()_+</t>
+  </si>
+  <si>
+    <t>VERIFYSEARCHRESULTS</t>
+  </si>
+  <si>
+    <t>searchError</t>
+  </si>
+  <si>
+    <t>Search - My Store</t>
+  </si>
+  <si>
+    <t>No results</t>
+  </si>
+  <si>
+    <t>TC # 01.06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,19 +518,19 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -544,18 +547,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -563,117 +566,123 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="7" t="s">
         <v>6</v>
@@ -683,7 +692,10 @@
       <c r="E11" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Sign Up Err Handl TC, refactor UIOperation class
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10872" windowHeight="4968" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="4965" tabRatio="331"/>
   </bookViews>
   <sheets>
     <sheet name="ErrorHandling" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Keyword</t>
   </si>
@@ -67,40 +67,43 @@
     <t>SETTEXTIN</t>
   </si>
   <si>
-    <t>searchField</t>
-  </si>
-  <si>
-    <t>searchButton</t>
-  </si>
-  <si>
     <t>My Store</t>
   </si>
   <si>
-    <t>TC # 01.06 - Search can`t find results</t>
-  </si>
-  <si>
-    <t>~!@#$%^&amp;*()_+</t>
-  </si>
-  <si>
-    <t>VERIFYSEARCHRESULTS</t>
-  </si>
-  <si>
-    <t>searchError</t>
-  </si>
-  <si>
-    <t>Search - My Store</t>
-  </si>
-  <si>
-    <t>No results</t>
-  </si>
-  <si>
-    <t>TC # 01.06</t>
+    <t>TC # 01.02</t>
+  </si>
+  <si>
+    <t>loginButton</t>
+  </si>
+  <si>
+    <t>Login - My Store</t>
+  </si>
+  <si>
+    <t>newUserNameField</t>
+  </si>
+  <si>
+    <t>createAccountButton</t>
+  </si>
+  <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
+    <t>VERIFYERRORMESSAGE</t>
+  </si>
+  <si>
+    <t>createAccountError</t>
+  </si>
+  <si>
+    <t>Invalid email address.</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Handling Error During Sign Up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +162,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -197,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -205,11 +202,16 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -515,22 +517,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -547,31 +549,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
@@ -582,120 +584,132 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7" t="s">
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="11"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Handling Error when filling personal information (Create An Account) TC
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="62">
   <si>
     <t>Keyword</t>
   </si>
@@ -98,13 +98,115 @@
   </si>
   <si>
     <t>TC # 01.01 - Handling Error During Sign Up</t>
+  </si>
+  <si>
+    <t>SETUNIQUETEXTIN</t>
+  </si>
+  <si>
+    <t>volchanskij@gmail.com</t>
+  </si>
+  <si>
+    <t>CLICKRADIOBUTTON</t>
+  </si>
+  <si>
+    <t>genderRadioButton</t>
+  </si>
+  <si>
+    <t>firstNameTextField</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>lastNameTextField</t>
+  </si>
+  <si>
+    <t>bruno</t>
+  </si>
+  <si>
+    <t>newPasswordTextField</t>
+  </si>
+  <si>
+    <t>testPWD001</t>
+  </si>
+  <si>
+    <t>newAddressTextField</t>
+  </si>
+  <si>
+    <t>178 somwhere I belong</t>
+  </si>
+  <si>
+    <t>newCityTextField</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>CHOOSEFROM</t>
+  </si>
+  <si>
+    <t>stateDropDownMenu</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>newPostCodeTextField</t>
+  </si>
+  <si>
+    <t>newMobilePhoneTextField</t>
+  </si>
+  <si>
+    <t>registerAccountButton</t>
+  </si>
+  <si>
+    <t>My account - My Store</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Handling Error when filling personal information (Create An Account)</t>
+  </si>
+  <si>
+    <t>TC # 01.01</t>
+  </si>
+  <si>
+    <t>registerAccountError</t>
+  </si>
+  <si>
+    <t>You must register at least one phone number.</t>
+  </si>
+  <si>
+    <t>lastname is required.</t>
+  </si>
+  <si>
+    <t>firstname is required.</t>
+  </si>
+  <si>
+    <t>passwd is required.</t>
+  </si>
+  <si>
+    <t>address1 is required.</t>
+  </si>
+  <si>
+    <t>city is required.</t>
+  </si>
+  <si>
+    <t>The Zip/Postal code you've entered is invalid. It must follow this format: 00000</t>
+  </si>
+  <si>
+    <t>This country requires you to choose a State.</t>
+  </si>
+  <si>
+    <t>94108</t>
+  </si>
+  <si>
+    <t>4158695625</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +243,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -212,6 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -517,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +638,7 @@
     <col min="2" max="2" width="25.28515625" style="7" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="39.140625" customWidth="1"/>
+    <col min="5" max="5" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -560,7 +669,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -573,7 +682,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
@@ -590,7 +699,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>10</v>
@@ -605,7 +714,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>9</v>
@@ -622,7 +731,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>12</v>
@@ -637,7 +746,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>14</v>
@@ -652,7 +761,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>16</v>
@@ -669,7 +778,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>10</v>
@@ -684,7 +793,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>24</v>
@@ -707,6 +816,617 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add Log In Err Handl TC
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="69">
   <si>
     <t>Keyword</t>
   </si>
@@ -200,6 +200,27 @@
   </si>
   <si>
     <t>4158695625</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Handling Error During Log In</t>
+  </si>
+  <si>
+    <t>TC # 01.03</t>
+  </si>
+  <si>
+    <t>usernameField</t>
+  </si>
+  <si>
+    <t>passwordField</t>
+  </si>
+  <si>
+    <t>shopLoginButton</t>
+  </si>
+  <si>
+    <t>An email address required.</t>
+  </si>
+  <si>
+    <t>Password is required.</t>
   </si>
 </sst>
 </file>
@@ -254,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -321,6 +348,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -626,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,8 +1458,251 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E61" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>